<commit_message>
Les fichiers propriétaires sont en PDF
</commit_message>
<xml_diff>
--- a/Documentation/Use cases et scenarii.xlsx
+++ b/Documentation/Use cases et scenarii.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timothee.RAPIN\OneDrive - CPNV\Documents\3emeAnnee\ProjetCSharp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timothee.RAPIN\OneDrive - CPNV\Documents\3emeAnnee\ProjetCSharp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Use cases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="Scénario - Rechercher une image" sheetId="7" r:id="rId7"/>
     <sheet name="Scénario - Telecharger une ima." sheetId="8" r:id="rId8"/>
     <sheet name="Scénario - Signialer une image" sheetId="9" r:id="rId9"/>
-    <sheet name="Scénario - s'abonner à un util." sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="62">
   <si>
     <t>Ajouter une image</t>
   </si>
@@ -51,9 +50,6 @@
   </si>
   <si>
     <t>Signialer une image</t>
-  </si>
-  <si>
-    <t>S'abonner à un utilisateur</t>
   </si>
   <si>
     <t>Identifiant + Titre</t>
@@ -473,37 +469,6 @@
   </si>
   <si>
     <t>L'image est signialée</t>
-  </si>
-  <si>
-    <t>M'abonner à un utilisateur</t>
-  </si>
-  <si>
-    <t>voir les images publiées par un utilisateur</t>
-  </si>
-  <si>
-    <t>Cliquer sur le nom de l'utilisateur qui l'a publiée</t>
-  </si>
-  <si>
-    <t>L'utilisateur apparait</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Cliquer sur </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[Suivre]</t>
-    </r>
-  </si>
-  <si>
-    <t>L'utilisateur est suivi</t>
   </si>
 </sst>
 </file>
@@ -596,12 +561,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,8 +607,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6766560" y="861060"/>
-          <a:ext cx="1181100" cy="1653540"/>
+          <a:off x="6736080" y="861060"/>
+          <a:ext cx="1176020" cy="1653540"/>
           <a:chOff x="6766560" y="647700"/>
           <a:chExt cx="1181100" cy="1630680"/>
         </a:xfrm>
@@ -914,8 +880,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1783080" y="822960"/>
-          <a:ext cx="1181100" cy="1653540"/>
+          <a:off x="1772920" y="822960"/>
+          <a:ext cx="1176020" cy="1653540"/>
           <a:chOff x="6766560" y="647700"/>
           <a:chExt cx="1181100" cy="1630680"/>
         </a:xfrm>
@@ -1289,55 +1255,6 @@
         <a:xfrm flipH="1">
           <a:off x="5722620" y="1265846"/>
           <a:ext cx="1043940" cy="1469734"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1744980</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>145706</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="37" name="Connecteur droit avec flèche 36"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="2" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="5707380" y="1265846"/>
-          <a:ext cx="1059180" cy="1865974"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1729,8 +1646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F1:F18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1741,13 +1658,13 @@
     <row r="1" spans="6:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="6:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="6:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="6:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="6:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1786,134 +1703,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="6:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="6:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="1" t="s">
-        <v>6</v>
-      </c>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="74" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1921,7 +1717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -1936,10 +1732,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -1947,10 +1743,10 @@
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1958,10 +1754,10 @@
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1969,10 +1765,10 @@
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1980,10 +1776,10 @@
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1993,31 +1789,31 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -2026,15 +1822,16 @@
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="58" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2042,7 +1839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
@@ -2057,10 +1854,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2068,10 +1865,10 @@
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2079,10 +1876,10 @@
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -2090,10 +1887,10 @@
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2101,10 +1898,10 @@
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2114,31 +1911,31 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -2147,15 +1944,16 @@
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="77" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2163,7 +1961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
@@ -2178,10 +1976,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2189,10 +1987,10 @@
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2200,7 +1998,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -2211,10 +2009,10 @@
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2222,10 +2020,10 @@
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2235,67 +2033,67 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2303,7 +2101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2318,10 +2116,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2329,10 +2127,10 @@
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2340,7 +2138,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
@@ -2351,10 +2149,10 @@
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2362,10 +2160,10 @@
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2375,28 +2173,29 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="53" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2404,7 +2203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2419,10 +2218,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2430,10 +2229,10 @@
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2441,7 +2240,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
@@ -2452,10 +2251,10 @@
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2463,10 +2262,10 @@
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2476,35 +2275,36 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="46" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2512,7 +2312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2527,10 +2327,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2538,10 +2338,10 @@
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2549,7 +2349,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -2560,10 +2360,10 @@
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2571,10 +2371,10 @@
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2584,37 +2384,38 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2622,7 +2423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2637,10 +2438,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2648,10 +2449,10 @@
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2659,7 +2460,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -2670,10 +2471,10 @@
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2681,10 +2482,10 @@
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2694,37 +2495,38 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2732,7 +2534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2747,10 +2549,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2758,10 +2560,10 @@
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2769,7 +2571,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -2780,10 +2582,10 @@
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2791,10 +2593,10 @@
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2804,36 +2606,37 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="46" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Scénarii (Ajout des cas critiques)
</commit_message>
<xml_diff>
--- a/Documentation/Use cases et scenarii.xlsx
+++ b/Documentation/Use cases et scenarii.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Use cases" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="83">
   <si>
     <t>Ajouter une image</t>
   </si>
@@ -469,6 +469,69 @@
   </si>
   <si>
     <t>L'image est signialée</t>
+  </si>
+  <si>
+    <t>Affiche une erreur "Tout les champs doivent être remplis"</t>
+  </si>
+  <si>
+    <t>Le format de l'adresse mail est incorrect</t>
+  </si>
+  <si>
+    <t>Affiche une erreur "L'adresse mail est incorrect"</t>
+  </si>
+  <si>
+    <t>Le mot de passe à moins de 8 charactères</t>
+  </si>
+  <si>
+    <t>Affiche une erreur "Le mot de passe doit avoir 8 charactères minimum"</t>
+  </si>
+  <si>
+    <t>mail incorrect</t>
+  </si>
+  <si>
+    <t>Affiche l'erreur "Mail ou mot de passe incorrect"</t>
+  </si>
+  <si>
+    <t>mot de passe incorrect</t>
+  </si>
+  <si>
+    <t>Affiche l'erreur "Il manque un titre"</t>
+  </si>
+  <si>
+    <t>Ajouter une image et une description</t>
+  </si>
+  <si>
+    <t>Ajouter un titre et une description</t>
+  </si>
+  <si>
+    <t>Ajouter un titre et une image</t>
+  </si>
+  <si>
+    <t>Affiche l'erreur "Il manque une image"</t>
+  </si>
+  <si>
+    <t>Affiche l'erreur "Il manque une description"</t>
+  </si>
+  <si>
+    <t>Image trop volumineuse</t>
+  </si>
+  <si>
+    <t>Affiche l'erreur "Image trop volumineuse"</t>
+  </si>
+  <si>
+    <t>Image trop petite</t>
+  </si>
+  <si>
+    <t>Affiche l'erreur "Image trop petite"</t>
+  </si>
+  <si>
+    <t>Format incorrect</t>
+  </si>
+  <si>
+    <t>Affiche l'erreur "Le format de l'image est incorrect"</t>
+  </si>
+  <si>
+    <t>Cliquer sur L'icon "loupe"</t>
   </si>
 </sst>
 </file>
@@ -607,8 +670,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6736080" y="861060"/>
-          <a:ext cx="1176020" cy="1653540"/>
+          <a:off x="6909487" y="856735"/>
+          <a:ext cx="1206842" cy="1645509"/>
           <a:chOff x="6766560" y="647700"/>
           <a:chExt cx="1181100" cy="1630680"/>
         </a:xfrm>
@@ -880,8 +943,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1772920" y="822960"/>
-          <a:ext cx="1176020" cy="1653540"/>
+          <a:off x="1820562" y="819665"/>
+          <a:ext cx="1206844" cy="1643449"/>
           <a:chOff x="6766560" y="647700"/>
           <a:chExt cx="1181100" cy="1630680"/>
         </a:xfrm>
@@ -1646,7 +1709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F1:F18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -1715,10 +1778,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1726,8 +1789,8 @@
     <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1813,19 +1876,74 @@
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1837,10 +1955,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:E9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1848,8 +1966,8 @@
     <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1937,7 +2055,9 @@
       <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1948,6 +2068,48 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1959,10 +2121,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:E11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1970,7 +2132,7 @@
     <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="50.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2076,18 +2238,132 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="3" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2101,7 +2377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2203,7 +2479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2310,9 +2586,129 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2352,7 +2748,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -2363,7 +2759,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2397,20 +2793,20 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2419,11 +2815,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2452,7 +2848,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2463,7 +2859,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -2474,7 +2870,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2517,117 +2913,6 @@
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C8" s="3" t="s">
         <v>60</v>
       </c>
       <c r="D8" s="3"/>

</xml_diff>